<commit_message>
report with password added
</commit_message>
<xml_diff>
--- a/api/informe.xlsx
+++ b/api/informe.xlsx
@@ -15,12 +15,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Total Trabajado</t>
+  </si>
+  <si>
+    <t>2022-04-24</t>
+  </si>
+  <si>
+    <t>2022-04-25</t>
+  </si>
+  <si>
+    <t>2022-04-26</t>
+  </si>
   <si>
     <t>Ana Tia</t>
   </si>
   <si>
+    <t>07:02:25</t>
+  </si>
+  <si>
+    <t>04:00:00</t>
+  </si>
+  <si>
+    <t>00:02:15</t>
+  </si>
+  <si>
+    <t>03:00:10</t>
+  </si>
+  <si>
     <t>Pepe Hongo</t>
+  </si>
+  <si>
+    <t>08:00:44</t>
+  </si>
+  <si>
+    <t>Pepito Hongo</t>
+  </si>
+  <si>
+    <t>02:00:00</t>
+  </si>
+  <si>
+    <t>01:00:00</t>
+  </si>
+  <si>
+    <t>00:00:14</t>
+  </si>
+  <si>
+    <t>Pablo Sobrino</t>
+  </si>
+  <si>
+    <t>00:00:13</t>
   </si>
 </sst>
 </file>
@@ -28,9 +76,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -53,9 +110,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -356,31 +422,95 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="3"/>
+    <col min="3" max="3" width="12" bestFit="true" customWidth="true" style="3"/>
+    <col min="4" max="4" width="12" bestFit="true" customWidth="true" style="3"/>
+    <col min="5" max="5" width="12" bestFit="true" customWidth="true" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5"/>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>